<commit_message>
explore human in loop flags
</commit_message>
<xml_diff>
--- a/2024-10-17_inland_water_quality_human_in_loop_tracking.xlsx
+++ b/2024-10-17_inland_water_quality_human_in_loop_tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicole Torrie\Documents\R\cmp_code\inland_thresholds_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39CE9703-0A63-418F-9AAA-330E0C36B81B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A97D88-9C71-42EE-868D-6E8CE9229E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-13275" windowWidth="29040" windowHeight="17520" xr2:uid="{D8B98A3C-11CD-483A-8C6D-31938E55AC89}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="35">
   <si>
     <t>station</t>
   </si>
@@ -108,40 +108,40 @@
     <t>string was entangled in fishing gear</t>
   </si>
   <si>
-    <t>LaHave 2</t>
-  </si>
-  <si>
-    <t>2023-Jun-20 to 2023-Oct-4</t>
-  </si>
-  <si>
-    <t>Liscomb 1</t>
-  </si>
-  <si>
     <t>2023-Jun-08 to 2023-Oct-11</t>
   </si>
   <si>
-    <t>Liscomb 2</t>
-  </si>
-  <si>
-    <t>Mersey 2</t>
-  </si>
-  <si>
     <t>2023-Jun-23 to 2023-Oct-13</t>
   </si>
   <si>
-    <t>Tusket 3</t>
-  </si>
-  <si>
     <t>2023-Jun-29 to 2023-Oct-18</t>
   </si>
   <si>
     <t>sensor loose from anchor upon retrieval</t>
   </si>
   <si>
-    <t>Middle 1</t>
-  </si>
-  <si>
     <t>2024-Jun-11 to 2024-Sep-29</t>
+  </si>
+  <si>
+    <t>LaHave River 2</t>
+  </si>
+  <si>
+    <t>Liscomb River 1</t>
+  </si>
+  <si>
+    <t>Liscomb River 2</t>
+  </si>
+  <si>
+    <t>Mersey River 2</t>
+  </si>
+  <si>
+    <t>Tusket River 3</t>
+  </si>
+  <si>
+    <t>Middle River 1</t>
+  </si>
+  <si>
+    <t>2023-Jun-20 to 2023-Oct-04</t>
   </si>
 </sst>
 </file>
@@ -188,7 +188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -201,6 +201,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -537,16 +543,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC401DDE-AE7E-4B2C-AD75-5A66A9319D76}">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.5546875" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.6640625" style="3" bestFit="1" customWidth="1"/>
@@ -564,7 +570,7 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -600,10 +606,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>24</v>
+        <v>28</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>9</v>
@@ -635,10 +641,10 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>9</v>
@@ -667,10 +673,10 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>9</v>
@@ -699,10 +705,10 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>9</v>
@@ -734,10 +740,10 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>9</v>
@@ -766,10 +772,10 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>9</v>
@@ -798,10 +804,10 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>26</v>
+        <v>30</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>9</v>
@@ -830,10 +836,10 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>26</v>
+        <v>30</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>9</v>
@@ -862,10 +868,10 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>26</v>
+        <v>30</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>9</v>
@@ -894,10 +900,10 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>9</v>
@@ -921,15 +927,15 @@
         <v>12</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>9</v>
@@ -958,10 +964,10 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>9</v>
@@ -989,8 +995,8 @@
       <c r="A14" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>34</v>
+      <c r="B14" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>9</v>
@@ -1017,7 +1023,15 @@
         <v>12</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>32</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>